<commit_message>
agregando datos de Excel al JSON
</commit_message>
<xml_diff>
--- a/data/empresas.xlsx
+++ b/data/empresas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\PROYECTOS y ESTUDIO\Proyectos\Legasa Filtros por checkbox(BACK Y FRONT)\BACKEND-DATOS-EXCEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A389486-3722-430A-A31F-BD7286ABA332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFFEDA5-936F-4406-A43A-EB8240D0ABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Registro</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>harina extruida de maca, quinua, cañihua</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>harinas extruida de maca, maca, ajonjolí</t>
+  </si>
+  <si>
+    <t>harina extruidas de maca, avena, anís</t>
   </si>
 </sst>
 </file>
@@ -513,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,6 +715,39 @@
         <v>36</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>